<commit_message>
minor selector and config fixes
</commit_message>
<xml_diff>
--- a/src/resources/data/testData.xlsx
+++ b/src/resources/data/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Space\workspace\vscode-workspace\playwright-sample-project\src\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\node\playwright-sample-project\src\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0092195-DFC7-4250-B2E5-CD3662DBF2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AD55D1-A003-4843-B7B5-A637064473C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="734" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regression" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>Login with valid credentials</t>
   </si>
   <si>
-    <t>James</t>
-  </si>
-  <si>
     <t>Login with invalid credentials</t>
   </si>
   <si>
@@ -510,6 +507,9 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>JamesB</t>
   </si>
 </sst>
 </file>
@@ -562,14 +562,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -854,336 +852,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="6" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>133</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>157</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -1206,169 +971,169 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B64F1D3-BE77-42C5-8522-489964BC065B}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="1"/>
+    <col min="15" max="15" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>11235</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="H2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>11645</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="O3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1389,94 +1154,94 @@
       <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.5703125" customWidth="1"/>
-    <col min="8" max="8" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.5546875" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
         <v>98</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
         <v>99</v>
       </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>100</v>
       </c>
-      <c r="H1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2">
         <v>1337</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>110</v>
+      <c r="G2" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="H2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3">
         <v>1547</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E3" t="s">
-        <v>104</v>
-      </c>
-      <c r="F3" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" t="s">
         <v>108</v>
-      </c>
-      <c r="H3" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1493,25 +1258,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A954124-2682-439B-BF75-C124F90C5D43}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1523,12 +1288,12 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>1243</v>
@@ -1537,47 +1302,47 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>158</v>
       </c>
       <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>16</v>
       </c>
       <c r="B3">
         <v>1244</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
       <c r="F3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4">
         <v>1245</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>158</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1594,191 +1359,191 @@
       <selection activeCell="B1" sqref="B1:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
         <v>58</v>
       </c>
-      <c r="F1" t="s">
-        <v>59</v>
-      </c>
       <c r="G1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" t="s">
         <v>70</v>
       </c>
-      <c r="H1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2">
         <v>1137</v>
       </c>
       <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
         <v>64</v>
       </c>
-      <c r="D2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="5"/>
+      <c r="E2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="4"/>
       <c r="G2">
         <v>200</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3">
         <v>1138</v>
       </c>
       <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
         <v>67</v>
       </c>
-      <c r="D3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" s="5"/>
+      <c r="E3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="4"/>
       <c r="G3">
         <v>200</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4">
         <v>1139</v>
       </c>
       <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
         <v>76</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" t="s">
         <v>77</v>
-      </c>
-      <c r="E4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" t="s">
-        <v>78</v>
       </c>
       <c r="G4">
         <v>200</v>
       </c>
       <c r="H4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>80</v>
       </c>
       <c r="B5">
         <v>1140</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" t="s">
         <v>81</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F5" t="s">
-        <v>82</v>
       </c>
       <c r="G5">
         <v>200</v>
       </c>
       <c r="H5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6">
         <v>1141</v>
       </c>
       <c r="C6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" t="s">
         <v>86</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" t="s">
         <v>88</v>
-      </c>
-      <c r="F6" t="s">
-        <v>89</v>
       </c>
       <c r="G6">
         <v>200</v>
       </c>
       <c r="H6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>91</v>
       </c>
       <c r="B7">
         <v>1142</v>
       </c>
       <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" t="s">
         <v>92</v>
       </c>
-      <c r="D7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>74</v>
+      <c r="E7" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="G7">
         <v>200</v>
       </c>
       <c r="H7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1795,146 +1560,146 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
         <v>60</v>
       </c>
-      <c r="E1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" t="s">
-        <v>61</v>
-      </c>
       <c r="H1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2">
         <v>1113</v>
       </c>
       <c r="C2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>136</v>
       </c>
       <c r="G2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" t="s">
         <v>140</v>
       </c>
-      <c r="H2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3">
         <v>1114</v>
       </c>
       <c r="C3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H3" t="s">
         <v>146</v>
       </c>
-      <c r="D3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="G3" t="s">
-        <v>140</v>
-      </c>
-      <c r="H3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B4">
         <v>1115</v>
       </c>
       <c r="C4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="G4" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" t="s">
         <v>151</v>
       </c>
-      <c r="D4" t="s">
-        <v>148</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="G4" t="s">
-        <v>140</v>
-      </c>
-      <c r="H4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B5">
         <v>1116</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>154</v>
-      </c>
       <c r="G5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" t="s">
         <v>138</v>
-      </c>
-      <c r="H5" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1955,125 +1720,125 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="102.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="102.44140625" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>114</v>
       </c>
       <c r="B2">
         <v>1467</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3">
         <v>1468</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D3" s="7" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4">
         <v>1469</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5">
         <v>1470</v>
       </c>
       <c r="C5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6">
         <v>1471</v>
       </c>
       <c r="C6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>129</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>130</v>
       </c>
       <c r="B7">
         <v>1472</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B8">
         <v>1473</v>
       </c>
       <c r="C8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Disabled REST test from Regression test  suite
</commit_message>
<xml_diff>
--- a/src/resources/data/testData.xlsx
+++ b/src/resources/data/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\node\playwright-sample-project\src\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84D6278-6E4E-4B6D-80AA-B47086BEA87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1622573F-2255-46ED-AAE4-CD193D47F7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="734" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regression" sheetId="1" r:id="rId1"/>
@@ -854,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -903,7 +903,7 @@
         <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -1355,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9496EF85-5873-4562-AF45-3630E5F53D1F}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>